<commit_message>
Přidání dokumentu 3 iterace.
</commit_message>
<xml_diff>
--- a/Ostatní/Vykaz prace.xlsx
+++ b/Ostatní/Vykaz prace.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="100">
   <si>
     <t>Beránek Petr</t>
   </si>
@@ -301,6 +301,21 @@
   </si>
   <si>
     <t>Oprava scénařů u USE-CASE</t>
+  </si>
+  <si>
+    <t>Oprava scénářů a dalších chyb.</t>
+  </si>
+  <si>
+    <t>Generování diagramů a úprava vsledné dokumentace</t>
+  </si>
+  <si>
+    <t>Úprava šablon pro generování dokumentace</t>
+  </si>
+  <si>
+    <t>Vytvoření databázového modelu</t>
+  </si>
+  <si>
+    <t>Oponentura k druhé iteraci</t>
   </si>
 </sst>
 </file>
@@ -325,7 +340,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="36">
+  <borders count="39">
     <border>
       <left/>
       <right/>
@@ -796,11 +811,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -893,6 +945,24 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -911,23 +981,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1228,10 +1293,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K35"/>
+  <dimension ref="A1:K37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="K33" sqref="K33"/>
+    <sheetView tabSelected="1" topLeftCell="D29" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I34" sqref="I34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="42.6" customHeight="1"/>
@@ -1252,26 +1317,26 @@
   <sheetData>
     <row r="1" spans="1:11" ht="15.75" customHeight="1" thickBot="1">
       <c r="A1" s="9"/>
-      <c r="B1" s="38" t="s">
+      <c r="B1" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="39"/>
-      <c r="D1" s="36" t="s">
+      <c r="C1" s="45"/>
+      <c r="D1" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="37"/>
-      <c r="F1" s="40" t="s">
+      <c r="E1" s="43"/>
+      <c r="F1" s="46" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="41"/>
-      <c r="H1" s="36" t="s">
+      <c r="G1" s="47"/>
+      <c r="H1" s="42" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="37"/>
-      <c r="J1" s="40" t="s">
+      <c r="I1" s="43"/>
+      <c r="J1" s="46" t="s">
         <v>69</v>
       </c>
-      <c r="K1" s="41"/>
+      <c r="K1" s="47"/>
     </row>
     <row r="2" spans="1:11" ht="30.75" thickBot="1">
       <c r="A2" s="2" t="s">
@@ -1309,7 +1374,7 @@
       </c>
     </row>
     <row r="3" spans="1:11" ht="42.6" customHeight="1">
-      <c r="A3" s="45" t="s">
+      <c r="A3" s="39" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="8">
@@ -1344,7 +1409,7 @@
       </c>
     </row>
     <row r="4" spans="1:11" ht="42.6" customHeight="1">
-      <c r="A4" s="47"/>
+      <c r="A4" s="41"/>
       <c r="B4" s="14"/>
       <c r="C4" s="24"/>
       <c r="D4" s="25"/>
@@ -1365,7 +1430,7 @@
       </c>
     </row>
     <row r="5" spans="1:11" ht="42.6" customHeight="1" thickBot="1">
-      <c r="A5" s="46"/>
+      <c r="A5" s="40"/>
       <c r="B5" s="6"/>
       <c r="C5" s="26"/>
       <c r="D5" s="27"/>
@@ -1382,7 +1447,7 @@
       <c r="K5" s="7"/>
     </row>
     <row r="6" spans="1:11" ht="42.6" customHeight="1">
-      <c r="A6" s="45" t="s">
+      <c r="A6" s="39" t="s">
         <v>22</v>
       </c>
       <c r="B6" s="12">
@@ -1417,7 +1482,7 @@
       </c>
     </row>
     <row r="7" spans="1:11" ht="42.6" customHeight="1">
-      <c r="A7" s="47"/>
+      <c r="A7" s="41"/>
       <c r="B7" s="4">
         <v>2.5</v>
       </c>
@@ -1434,7 +1499,7 @@
       <c r="K7" s="5"/>
     </row>
     <row r="8" spans="1:11" ht="42.6" customHeight="1" thickBot="1">
-      <c r="A8" s="46"/>
+      <c r="A8" s="40"/>
       <c r="B8" s="6">
         <v>0.75</v>
       </c>
@@ -1451,7 +1516,7 @@
       <c r="K8" s="7"/>
     </row>
     <row r="9" spans="1:11" ht="42.6" customHeight="1">
-      <c r="A9" s="45" t="s">
+      <c r="A9" s="39" t="s">
         <v>21</v>
       </c>
       <c r="B9" s="12">
@@ -1486,7 +1551,7 @@
       </c>
     </row>
     <row r="10" spans="1:11" ht="42.6" customHeight="1">
-      <c r="A10" s="47"/>
+      <c r="A10" s="41"/>
       <c r="B10" s="4">
         <v>3.25</v>
       </c>
@@ -1507,7 +1572,7 @@
       </c>
     </row>
     <row r="11" spans="1:11" ht="42.6" customHeight="1">
-      <c r="A11" s="47"/>
+      <c r="A11" s="41"/>
       <c r="B11" s="4">
         <v>2</v>
       </c>
@@ -1524,7 +1589,7 @@
       <c r="K11" s="5"/>
     </row>
     <row r="12" spans="1:11" ht="42.6" customHeight="1" thickBot="1">
-      <c r="A12" s="46"/>
+      <c r="A12" s="40"/>
       <c r="B12" s="6">
         <v>3</v>
       </c>
@@ -1541,7 +1606,7 @@
       <c r="K12" s="7"/>
     </row>
     <row r="13" spans="1:11" ht="42.6" customHeight="1">
-      <c r="A13" s="45" t="s">
+      <c r="A13" s="39" t="s">
         <v>20</v>
       </c>
       <c r="B13" s="12">
@@ -1576,7 +1641,7 @@
       </c>
     </row>
     <row r="14" spans="1:11" ht="42.6" customHeight="1" thickBot="1">
-      <c r="A14" s="46"/>
+      <c r="A14" s="40"/>
       <c r="B14" s="6">
         <v>4.5</v>
       </c>
@@ -1601,7 +1666,7 @@
       </c>
     </row>
     <row r="15" spans="1:11" ht="42.6" customHeight="1">
-      <c r="A15" s="45" t="s">
+      <c r="A15" s="39" t="s">
         <v>29</v>
       </c>
       <c r="B15" s="12">
@@ -1636,7 +1701,7 @@
       </c>
     </row>
     <row r="16" spans="1:11" ht="42.6" customHeight="1">
-      <c r="A16" s="47"/>
+      <c r="A16" s="41"/>
       <c r="B16" s="4">
         <v>4.5</v>
       </c>
@@ -1669,7 +1734,7 @@
       </c>
     </row>
     <row r="17" spans="1:11" ht="42.6" customHeight="1">
-      <c r="A17" s="47"/>
+      <c r="A17" s="41"/>
       <c r="B17" s="4"/>
       <c r="C17" s="24"/>
       <c r="D17" s="4"/>
@@ -1694,7 +1759,7 @@
       </c>
     </row>
     <row r="18" spans="1:11" ht="42.6" customHeight="1">
-      <c r="A18" s="47"/>
+      <c r="A18" s="41"/>
       <c r="B18" s="4"/>
       <c r="C18" s="24"/>
       <c r="D18" s="4"/>
@@ -1715,7 +1780,7 @@
       </c>
     </row>
     <row r="19" spans="1:11" ht="42.6" customHeight="1">
-      <c r="A19" s="47"/>
+      <c r="A19" s="41"/>
       <c r="B19" s="4"/>
       <c r="C19" s="24"/>
       <c r="D19" s="4"/>
@@ -1736,7 +1801,7 @@
       </c>
     </row>
     <row r="20" spans="1:11" ht="42.6" customHeight="1">
-      <c r="A20" s="47"/>
+      <c r="A20" s="41"/>
       <c r="B20" s="4"/>
       <c r="C20" s="24"/>
       <c r="D20" s="4"/>
@@ -1753,7 +1818,7 @@
       <c r="K20" s="5"/>
     </row>
     <row r="21" spans="1:11" ht="42.6" customHeight="1" thickBot="1">
-      <c r="A21" s="46"/>
+      <c r="A21" s="40"/>
       <c r="B21" s="6"/>
       <c r="C21" s="26"/>
       <c r="D21" s="6"/>
@@ -1800,7 +1865,7 @@
       <c r="K22" s="11"/>
     </row>
     <row r="23" spans="1:11" ht="42.6" customHeight="1" thickBot="1">
-      <c r="A23" s="42" t="s">
+      <c r="A23" s="36" t="s">
         <v>65</v>
       </c>
       <c r="B23" s="12">
@@ -1827,7 +1892,7 @@
       </c>
     </row>
     <row r="24" spans="1:11" ht="42.6" customHeight="1" thickBot="1">
-      <c r="A24" s="42"/>
+      <c r="A24" s="36"/>
       <c r="B24" s="6">
         <v>2.5</v>
       </c>
@@ -1844,7 +1909,7 @@
       <c r="K24" s="7"/>
     </row>
     <row r="25" spans="1:11" ht="42.6" customHeight="1" thickBot="1">
-      <c r="A25" s="42" t="s">
+      <c r="A25" s="36" t="s">
         <v>67</v>
       </c>
       <c r="B25" s="12">
@@ -1875,7 +1940,7 @@
       </c>
     </row>
     <row r="26" spans="1:11" ht="42.6" customHeight="1" thickBot="1">
-      <c r="A26" s="42"/>
+      <c r="A26" s="36"/>
       <c r="B26" s="10"/>
       <c r="C26" s="35"/>
       <c r="D26" s="10"/>
@@ -1892,7 +1957,7 @@
       <c r="K26" s="11"/>
     </row>
     <row r="27" spans="1:11" ht="42.6" customHeight="1" thickBot="1">
-      <c r="A27" s="42"/>
+      <c r="A27" s="36"/>
       <c r="B27" s="6"/>
       <c r="C27" s="30"/>
       <c r="D27" s="6"/>
@@ -1941,8 +2006,8 @@
       </c>
       <c r="K28" s="32"/>
     </row>
-    <row r="29" spans="1:11" ht="42.6" customHeight="1">
-      <c r="A29" s="43" t="s">
+    <row r="29" spans="1:11" ht="42.6" customHeight="1" thickBot="1">
+      <c r="A29" s="37" t="s">
         <v>72</v>
       </c>
       <c r="B29" s="12">
@@ -1959,8 +2024,12 @@
       </c>
       <c r="F29" s="12"/>
       <c r="G29" s="13"/>
-      <c r="H29" s="12"/>
-      <c r="I29" s="13"/>
+      <c r="H29" s="12">
+        <v>2</v>
+      </c>
+      <c r="I29" s="13" t="s">
+        <v>95</v>
+      </c>
       <c r="J29" s="12">
         <v>1.75</v>
       </c>
@@ -1969,7 +2038,7 @@
       </c>
     </row>
     <row r="30" spans="1:11" ht="42.6" customHeight="1" thickBot="1">
-      <c r="A30" s="44"/>
+      <c r="A30" s="38"/>
       <c r="B30" s="6">
         <v>2</v>
       </c>
@@ -1980,8 +2049,12 @@
       <c r="E30" s="7"/>
       <c r="F30" s="6"/>
       <c r="G30" s="7"/>
-      <c r="H30" s="6"/>
-      <c r="I30" s="7"/>
+      <c r="H30" s="16">
+        <v>3</v>
+      </c>
+      <c r="I30" s="32" t="s">
+        <v>97</v>
+      </c>
       <c r="J30" s="6">
         <v>5</v>
       </c>
@@ -1990,136 +2063,179 @@
       </c>
     </row>
     <row r="31" spans="1:11" ht="42.6" customHeight="1" thickBot="1">
-      <c r="A31" s="33" t="s">
+      <c r="A31" s="48"/>
+      <c r="B31" s="49"/>
+      <c r="C31" s="50"/>
+      <c r="D31" s="49"/>
+      <c r="E31" s="51"/>
+      <c r="F31" s="49"/>
+      <c r="G31" s="52"/>
+      <c r="H31" s="6">
+        <v>10</v>
+      </c>
+      <c r="I31" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="J31" s="49"/>
+      <c r="K31" s="52"/>
+    </row>
+    <row r="32" spans="1:11" ht="42.6" customHeight="1" thickBot="1">
+      <c r="A32" s="48"/>
+      <c r="B32" s="49"/>
+      <c r="C32" s="50"/>
+      <c r="D32" s="49"/>
+      <c r="E32" s="51"/>
+      <c r="F32" s="49"/>
+      <c r="G32" s="52"/>
+      <c r="H32" s="49">
+        <v>7</v>
+      </c>
+      <c r="I32" s="52" t="s">
+        <v>98</v>
+      </c>
+      <c r="J32" s="49"/>
+      <c r="K32" s="52"/>
+    </row>
+    <row r="33" spans="1:11" ht="42.6" customHeight="1" thickBot="1">
+      <c r="A33" s="33" t="s">
         <v>73</v>
       </c>
-      <c r="B31" s="16">
+      <c r="B33" s="16">
         <v>5.25</v>
       </c>
-      <c r="C31" s="34" t="s">
+      <c r="C33" s="34" t="s">
         <v>81</v>
       </c>
-      <c r="D31" s="16">
+      <c r="D33" s="16">
         <v>6</v>
       </c>
-      <c r="E31" s="20" t="s">
+      <c r="E33" s="20" t="s">
         <v>75</v>
       </c>
-      <c r="F31" s="16"/>
-      <c r="G31" s="32"/>
-      <c r="H31" s="16"/>
-      <c r="I31" s="32"/>
-      <c r="J31" s="16">
+      <c r="F33" s="16"/>
+      <c r="G33" s="32"/>
+      <c r="H33" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="I33" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="J33" s="16">
         <v>11.5</v>
       </c>
-      <c r="K31" s="32" t="s">
+      <c r="K33" s="32" t="s">
         <v>92</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" ht="42.6" customHeight="1" thickBot="1">
-      <c r="A32" s="15" t="s">
-        <v>82</v>
-      </c>
-      <c r="B32" s="16">
-        <f>SUM(B28:B31)</f>
-        <v>51.75</v>
-      </c>
-      <c r="C32" s="32"/>
-      <c r="D32" s="16">
-        <f>SUM(D28:D31)</f>
-        <v>28.5</v>
-      </c>
-      <c r="E32" s="32"/>
-      <c r="F32" s="16">
-        <f>SUM(F28:F31)</f>
-        <v>28.75</v>
-      </c>
-      <c r="G32" s="32"/>
-      <c r="H32" s="16">
-        <f>SUM(H28:H31)</f>
-        <v>19.25</v>
-      </c>
-      <c r="I32" s="32"/>
-      <c r="J32" s="16">
-        <f>SUM(J28:J31)</f>
-        <v>46</v>
-      </c>
-      <c r="K32" s="32"/>
-    </row>
-    <row r="33" spans="1:11" ht="42.6" customHeight="1" thickBot="1">
-      <c r="A33" s="15" t="s">
-        <v>83</v>
-      </c>
-      <c r="B33" s="16">
-        <v>0.25</v>
-      </c>
-      <c r="C33" s="32" t="s">
-        <v>84</v>
-      </c>
-      <c r="D33" s="16"/>
-      <c r="E33" s="32"/>
-      <c r="F33" s="16">
-        <v>1</v>
-      </c>
-      <c r="G33" s="32" t="s">
-        <v>90</v>
-      </c>
-      <c r="H33" s="16"/>
-      <c r="I33" s="32"/>
-      <c r="J33" s="16">
-        <v>0.5</v>
-      </c>
-      <c r="K33" s="32" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="34" spans="1:11" ht="42.6" customHeight="1" thickBot="1">
       <c r="A34" s="15" t="s">
-        <v>85</v>
-      </c>
-      <c r="B34" s="16"/>
+        <v>82</v>
+      </c>
+      <c r="B34" s="16">
+        <f>SUM(B28:B33)</f>
+        <v>51.75</v>
+      </c>
       <c r="C34" s="32"/>
-      <c r="D34" s="16"/>
+      <c r="D34" s="16">
+        <f>SUM(D28:D33)</f>
+        <v>28.5</v>
+      </c>
       <c r="E34" s="32"/>
-      <c r="F34" s="16"/>
+      <c r="F34" s="16">
+        <f>SUM(F28:F33)</f>
+        <v>28.75</v>
+      </c>
       <c r="G34" s="32"/>
-      <c r="H34" s="16"/>
+      <c r="H34" s="16">
+        <f>SUM(H28:H31)</f>
+        <v>34.25</v>
+      </c>
       <c r="I34" s="32"/>
-      <c r="J34" s="16"/>
+      <c r="J34" s="16">
+        <f>SUM(J28:J33)</f>
+        <v>46</v>
+      </c>
       <c r="K34" s="32"/>
     </row>
     <row r="35" spans="1:11" ht="42.6" customHeight="1" thickBot="1">
       <c r="A35" s="15" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B35" s="16">
-        <f>SUM(B32:B34)</f>
-        <v>52</v>
-      </c>
-      <c r="C35" s="32"/>
-      <c r="D35" s="16">
-        <f>SUM(D32:D34)</f>
-        <v>28.5</v>
-      </c>
+        <v>0.25</v>
+      </c>
+      <c r="C35" s="32" t="s">
+        <v>84</v>
+      </c>
+      <c r="D35" s="16"/>
       <c r="E35" s="32"/>
       <c r="F35" s="16">
-        <f>SUM(F32:F34)</f>
-        <v>29.75</v>
-      </c>
-      <c r="G35" s="32"/>
-      <c r="H35" s="16">
-        <f>SUM(H32:H34)</f>
-        <v>19.25</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="G35" s="32" t="s">
+        <v>90</v>
+      </c>
+      <c r="H35" s="16"/>
       <c r="I35" s="32"/>
       <c r="J35" s="16">
-        <f>SUM(J32:J34)</f>
+        <v>0.5</v>
+      </c>
+      <c r="K35" s="32" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" ht="42.6" customHeight="1" thickBot="1">
+      <c r="A36" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="B36" s="16"/>
+      <c r="C36" s="32"/>
+      <c r="D36" s="16"/>
+      <c r="E36" s="32"/>
+      <c r="F36" s="16"/>
+      <c r="G36" s="32"/>
+      <c r="H36" s="16"/>
+      <c r="I36" s="32"/>
+      <c r="J36" s="16"/>
+      <c r="K36" s="32"/>
+    </row>
+    <row r="37" spans="1:11" ht="42.6" customHeight="1" thickBot="1">
+      <c r="A37" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="B37" s="16">
+        <f>SUM(B34:B36)</f>
+        <v>52</v>
+      </c>
+      <c r="C37" s="32"/>
+      <c r="D37" s="16">
+        <f>SUM(D34:D36)</f>
+        <v>28.5</v>
+      </c>
+      <c r="E37" s="32"/>
+      <c r="F37" s="16">
+        <f>SUM(F34:F36)</f>
+        <v>29.75</v>
+      </c>
+      <c r="G37" s="32"/>
+      <c r="H37" s="16">
+        <f>SUM(H34:H36)</f>
+        <v>34.25</v>
+      </c>
+      <c r="I37" s="32"/>
+      <c r="J37" s="16">
+        <f>SUM(J34:J36)</f>
         <v>46.5</v>
       </c>
-      <c r="K35" s="32"/>
+      <c r="K37" s="32"/>
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="J1:K1"/>
     <mergeCell ref="A23:A24"/>
     <mergeCell ref="A29:A30"/>
     <mergeCell ref="A13:A14"/>
@@ -2128,11 +2244,6 @@
     <mergeCell ref="A6:A8"/>
     <mergeCell ref="A9:A12"/>
     <mergeCell ref="A25:A27"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="H1:I1"/>
-    <mergeCell ref="J1:K1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Dokument 4. iterace plus přerozdělení bodů.
</commit_message>
<xml_diff>
--- a/Ostatní/Vykaz prace.xlsx
+++ b/Ostatní/Vykaz prace.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="315" yWindow="375" windowWidth="18825" windowHeight="7065"/>
@@ -11,12 +11,12 @@
     <sheet name="List2" sheetId="2" r:id="rId2"/>
     <sheet name="List3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="114">
   <si>
     <t>Beránek Petr</t>
   </si>
@@ -328,13 +328,43 @@
   </si>
   <si>
     <t>Java - příprava embedded databáze, hledání jak správně navrhnout a napsat DAO, vytvoření všech tříd, které budou jakkoliv pracovat s databází.</t>
+  </si>
+  <si>
+    <t>Oprava chyb v generování sekvenčních diagramů</t>
+  </si>
+  <si>
+    <t>Hledání, jak správně vytvořit Návrh tříd. Pokus o vytvoření návrhu jedné části.</t>
+  </si>
+  <si>
+    <t>Dopsání controllerů pro komunikaci GUI a databáze.</t>
+  </si>
+  <si>
+    <t>Sepsání uživatelského manuálu.</t>
+  </si>
+  <si>
+    <t>Sepsání zprávy o implementaci.</t>
+  </si>
+  <si>
+    <t>Oprava modelu nasazení</t>
+  </si>
+  <si>
+    <t>Generování konečné upravené dokumentace a úprava výsledného dokumentu.</t>
+  </si>
+  <si>
+    <t>Oprava databázového modelu dle oponentury</t>
+  </si>
+  <si>
+    <t>Celkem ze všech iterací</t>
+  </si>
+  <si>
+    <t>Vytvoření GUI</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -970,6 +1000,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -988,98 +1036,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normální" xfId="0" builtinId="0"/>
+    <cellStyle name="normální" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1089,14 +1051,14 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motiv systému Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motiv sady Office">
   <a:themeElements>
     <a:clrScheme name="Kancelář">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="0000FF"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="A7B4D1"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -1163,7 +1125,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -1198,7 +1159,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Kancelář">
@@ -1374,14 +1334,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K39"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:K42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="K42" sqref="K42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="42.6" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="42.6" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.140625" style="1" bestFit="1" customWidth="1"/>
@@ -1397,30 +1357,30 @@
     <col min="12" max="16384" width="8.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" ht="15.75" customHeight="1" thickBot="1">
       <c r="A1" s="9"/>
-      <c r="B1" s="43" t="s">
+      <c r="B1" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="44"/>
-      <c r="D1" s="41" t="s">
+      <c r="C1" s="50"/>
+      <c r="D1" s="47" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="42"/>
-      <c r="F1" s="45" t="s">
+      <c r="E1" s="48"/>
+      <c r="F1" s="51" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="46"/>
-      <c r="H1" s="41" t="s">
+      <c r="G1" s="52"/>
+      <c r="H1" s="47" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="42"/>
-      <c r="J1" s="45" t="s">
+      <c r="I1" s="48"/>
+      <c r="J1" s="51" t="s">
         <v>69</v>
       </c>
-      <c r="K1" s="46"/>
-    </row>
-    <row r="2" spans="1:11" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K1" s="52"/>
+    </row>
+    <row r="2" spans="1:11" ht="30.75" thickBot="1">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -1455,8 +1415,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="42.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="50" t="s">
+    <row r="3" spans="1:11" ht="42.6" customHeight="1">
+      <c r="A3" s="44" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="8">
@@ -1490,8 +1450,8 @@
         <v>44</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="42.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="52"/>
+    <row r="4" spans="1:11" ht="42.6" customHeight="1">
+      <c r="A4" s="46"/>
       <c r="B4" s="14"/>
       <c r="C4" s="24"/>
       <c r="D4" s="25"/>
@@ -1511,8 +1471,8 @@
         <v>45</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="42.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="51"/>
+    <row r="5" spans="1:11" ht="42.6" customHeight="1" thickBot="1">
+      <c r="A5" s="45"/>
       <c r="B5" s="6"/>
       <c r="C5" s="26"/>
       <c r="D5" s="27"/>
@@ -1528,8 +1488,8 @@
       <c r="J5" s="6"/>
       <c r="K5" s="7"/>
     </row>
-    <row r="6" spans="1:11" ht="42.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="50" t="s">
+    <row r="6" spans="1:11" ht="42.6" customHeight="1">
+      <c r="A6" s="44" t="s">
         <v>22</v>
       </c>
       <c r="B6" s="12">
@@ -1563,8 +1523,8 @@
         <v>46</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="42.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="52"/>
+    <row r="7" spans="1:11" ht="42.6" customHeight="1">
+      <c r="A7" s="46"/>
       <c r="B7" s="4">
         <v>2.5</v>
       </c>
@@ -1580,8 +1540,8 @@
       <c r="J7" s="4"/>
       <c r="K7" s="5"/>
     </row>
-    <row r="8" spans="1:11" ht="42.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="51"/>
+    <row r="8" spans="1:11" ht="42.6" customHeight="1" thickBot="1">
+      <c r="A8" s="45"/>
       <c r="B8" s="6">
         <v>0.75</v>
       </c>
@@ -1597,8 +1557,8 @@
       <c r="J8" s="6"/>
       <c r="K8" s="7"/>
     </row>
-    <row r="9" spans="1:11" ht="42.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="50" t="s">
+    <row r="9" spans="1:11" ht="42.6" customHeight="1">
+      <c r="A9" s="44" t="s">
         <v>21</v>
       </c>
       <c r="B9" s="12">
@@ -1632,8 +1592,8 @@
         <v>47</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="42.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="52"/>
+    <row r="10" spans="1:11" ht="42.6" customHeight="1">
+      <c r="A10" s="46"/>
       <c r="B10" s="4">
         <v>3.25</v>
       </c>
@@ -1653,8 +1613,8 @@
         <v>48</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="42.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="52"/>
+    <row r="11" spans="1:11" ht="42.6" customHeight="1">
+      <c r="A11" s="46"/>
       <c r="B11" s="4">
         <v>2</v>
       </c>
@@ -1670,8 +1630,8 @@
       <c r="J11" s="4"/>
       <c r="K11" s="5"/>
     </row>
-    <row r="12" spans="1:11" ht="42.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="51"/>
+    <row r="12" spans="1:11" ht="42.6" customHeight="1" thickBot="1">
+      <c r="A12" s="45"/>
       <c r="B12" s="6">
         <v>3</v>
       </c>
@@ -1687,8 +1647,8 @@
       <c r="J12" s="6"/>
       <c r="K12" s="7"/>
     </row>
-    <row r="13" spans="1:11" ht="42.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="50" t="s">
+    <row r="13" spans="1:11" ht="42.6" customHeight="1">
+      <c r="A13" s="44" t="s">
         <v>20</v>
       </c>
       <c r="B13" s="12">
@@ -1722,8 +1682,8 @@
         <v>49</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="42.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="51"/>
+    <row r="14" spans="1:11" ht="42.6" customHeight="1" thickBot="1">
+      <c r="A14" s="45"/>
       <c r="B14" s="6">
         <v>4.5</v>
       </c>
@@ -1747,8 +1707,8 @@
         <v>50</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="42.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="50" t="s">
+    <row r="15" spans="1:11" ht="42.6" customHeight="1">
+      <c r="A15" s="44" t="s">
         <v>29</v>
       </c>
       <c r="B15" s="12">
@@ -1782,8 +1742,8 @@
         <v>51</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="42.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="52"/>
+    <row r="16" spans="1:11" ht="42.6" customHeight="1">
+      <c r="A16" s="46"/>
       <c r="B16" s="4">
         <v>4.5</v>
       </c>
@@ -1815,8 +1775,8 @@
         <v>52</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="42.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="52"/>
+    <row r="17" spans="1:11" ht="42.6" customHeight="1">
+      <c r="A17" s="46"/>
       <c r="B17" s="4"/>
       <c r="C17" s="24"/>
       <c r="D17" s="4"/>
@@ -1840,8 +1800,8 @@
         <v>53</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="42.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="52"/>
+    <row r="18" spans="1:11" ht="42.6" customHeight="1">
+      <c r="A18" s="46"/>
       <c r="B18" s="4"/>
       <c r="C18" s="24"/>
       <c r="D18" s="4"/>
@@ -1861,8 +1821,8 @@
         <v>54</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="42.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="52"/>
+    <row r="19" spans="1:11" ht="42.6" customHeight="1">
+      <c r="A19" s="46"/>
       <c r="B19" s="4"/>
       <c r="C19" s="24"/>
       <c r="D19" s="4"/>
@@ -1882,8 +1842,8 @@
         <v>55</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="42.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="52"/>
+    <row r="20" spans="1:11" ht="42.6" customHeight="1">
+      <c r="A20" s="46"/>
       <c r="B20" s="4"/>
       <c r="C20" s="24"/>
       <c r="D20" s="4"/>
@@ -1899,8 +1859,8 @@
       <c r="J20" s="4"/>
       <c r="K20" s="5"/>
     </row>
-    <row r="21" spans="1:11" ht="42.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="51"/>
+    <row r="21" spans="1:11" ht="42.6" customHeight="1" thickBot="1">
+      <c r="A21" s="45"/>
       <c r="B21" s="6"/>
       <c r="C21" s="26"/>
       <c r="D21" s="6"/>
@@ -1916,7 +1876,7 @@
       <c r="J21" s="6"/>
       <c r="K21" s="7"/>
     </row>
-    <row r="22" spans="1:11" ht="42.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" ht="42.6" customHeight="1" thickBot="1">
       <c r="A22" s="3" t="s">
         <v>66</v>
       </c>
@@ -1946,8 +1906,8 @@
       </c>
       <c r="K22" s="11"/>
     </row>
-    <row r="23" spans="1:11" ht="42.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="47" t="s">
+    <row r="23" spans="1:11" ht="42.6" customHeight="1" thickBot="1">
+      <c r="A23" s="41" t="s">
         <v>65</v>
       </c>
       <c r="B23" s="12">
@@ -1973,8 +1933,8 @@
         <v>70</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="42.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="47"/>
+    <row r="24" spans="1:11" ht="42.6" customHeight="1" thickBot="1">
+      <c r="A24" s="41"/>
       <c r="B24" s="6">
         <v>2.5</v>
       </c>
@@ -1990,8 +1950,8 @@
       <c r="J24" s="6"/>
       <c r="K24" s="7"/>
     </row>
-    <row r="25" spans="1:11" ht="42.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="47" t="s">
+    <row r="25" spans="1:11" ht="42.6" customHeight="1" thickBot="1">
+      <c r="A25" s="41" t="s">
         <v>67</v>
       </c>
       <c r="B25" s="12">
@@ -2021,8 +1981,8 @@
         <v>71</v>
       </c>
     </row>
-    <row r="26" spans="1:11" ht="42.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="47"/>
+    <row r="26" spans="1:11" ht="42.6" customHeight="1" thickBot="1">
+      <c r="A26" s="41"/>
       <c r="B26" s="10"/>
       <c r="C26" s="35"/>
       <c r="D26" s="10"/>
@@ -2038,8 +1998,8 @@
       <c r="J26" s="10"/>
       <c r="K26" s="11"/>
     </row>
-    <row r="27" spans="1:11" ht="42.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="47"/>
+    <row r="27" spans="1:11" ht="42.6" customHeight="1" thickBot="1">
+      <c r="A27" s="41"/>
       <c r="B27" s="6"/>
       <c r="C27" s="30"/>
       <c r="D27" s="6"/>
@@ -2055,7 +2015,7 @@
       <c r="J27" s="6"/>
       <c r="K27" s="7"/>
     </row>
-    <row r="28" spans="1:11" ht="42.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" ht="42.6" customHeight="1" thickBot="1">
       <c r="A28" s="31" t="s">
         <v>68</v>
       </c>
@@ -2088,8 +2048,8 @@
       </c>
       <c r="K28" s="32"/>
     </row>
-    <row r="29" spans="1:11" ht="42.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="48" t="s">
+    <row r="29" spans="1:11" ht="42.6" customHeight="1" thickBot="1">
+      <c r="A29" s="42" t="s">
         <v>72</v>
       </c>
       <c r="B29" s="12">
@@ -2119,8 +2079,8 @@
         <v>91</v>
       </c>
     </row>
-    <row r="30" spans="1:11" ht="42.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="49"/>
+    <row r="30" spans="1:11" ht="42.6" customHeight="1" thickBot="1">
+      <c r="A30" s="43"/>
       <c r="B30" s="6">
         <v>2</v>
       </c>
@@ -2144,7 +2104,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="31" spans="1:11" ht="42.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11" ht="42.6" customHeight="1" thickBot="1">
       <c r="A31" s="36"/>
       <c r="B31" s="37"/>
       <c r="C31" s="38"/>
@@ -2161,7 +2121,7 @@
       <c r="J31" s="37"/>
       <c r="K31" s="40"/>
     </row>
-    <row r="32" spans="1:11" ht="42.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" ht="42.6" customHeight="1" thickBot="1">
       <c r="A32" s="36"/>
       <c r="B32" s="37"/>
       <c r="C32" s="38"/>
@@ -2178,7 +2138,7 @@
       <c r="J32" s="37"/>
       <c r="K32" s="40"/>
     </row>
-    <row r="33" spans="1:11" ht="42.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:11" ht="42.6" customHeight="1" thickBot="1">
       <c r="A33" s="33" t="s">
         <v>73</v>
       </c>
@@ -2209,7 +2169,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="34" spans="1:11" ht="42.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:11" ht="42.6" customHeight="1" thickBot="1">
       <c r="A34" s="15" t="s">
         <v>82</v>
       </c>
@@ -2239,7 +2199,7 @@
       </c>
       <c r="K34" s="32"/>
     </row>
-    <row r="35" spans="1:11" ht="42.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:11" ht="42.6" customHeight="1" thickBot="1">
       <c r="A35" s="15" t="s">
         <v>83</v>
       </c>
@@ -2257,8 +2217,12 @@
       <c r="G35" s="32" t="s">
         <v>90</v>
       </c>
-      <c r="H35" s="16"/>
-      <c r="I35" s="32"/>
+      <c r="H35" s="16">
+        <v>0.25</v>
+      </c>
+      <c r="I35" s="32" t="s">
+        <v>104</v>
+      </c>
       <c r="J35" s="16">
         <v>0.5</v>
       </c>
@@ -2266,7 +2230,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="36" spans="1:11" ht="42.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:11" ht="42.6" customHeight="1" thickBot="1">
       <c r="A36" s="15" t="s">
         <v>100</v>
       </c>
@@ -2280,12 +2244,20 @@
       <c r="E36" s="32"/>
       <c r="F36" s="16"/>
       <c r="G36" s="32"/>
-      <c r="H36" s="16"/>
-      <c r="I36" s="32"/>
-      <c r="J36" s="16"/>
-      <c r="K36" s="32"/>
-    </row>
-    <row r="37" spans="1:11" ht="42.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H36" s="16">
+        <v>2</v>
+      </c>
+      <c r="I36" s="32" t="s">
+        <v>111</v>
+      </c>
+      <c r="J36" s="16">
+        <v>0.5</v>
+      </c>
+      <c r="K36" s="32" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" ht="42.6" customHeight="1" thickBot="1">
       <c r="A37" s="15" t="s">
         <v>100</v>
       </c>
@@ -2299,62 +2271,142 @@
       <c r="E37" s="32"/>
       <c r="F37" s="16"/>
       <c r="G37" s="32"/>
-      <c r="H37" s="16"/>
-      <c r="I37" s="32"/>
-      <c r="J37" s="16"/>
-      <c r="K37" s="32"/>
-    </row>
-    <row r="38" spans="1:11" ht="42.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="15" t="s">
-        <v>85</v>
-      </c>
-      <c r="B38" s="16">
+      <c r="H37" s="16">
+        <v>3</v>
+      </c>
+      <c r="I37" s="32" t="s">
+        <v>105</v>
+      </c>
+      <c r="J37" s="16">
+        <v>4</v>
+      </c>
+      <c r="K37" s="32" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" ht="42.6" customHeight="1" thickBot="1">
+      <c r="A38" s="15"/>
+      <c r="B38" s="16"/>
+      <c r="C38" s="32"/>
+      <c r="D38" s="16">
         <v>10</v>
       </c>
-      <c r="C38" s="32" t="s">
-        <v>103</v>
-      </c>
-      <c r="D38" s="16"/>
-      <c r="E38" s="32"/>
+      <c r="E38" s="32" t="s">
+        <v>113</v>
+      </c>
       <c r="F38" s="16"/>
       <c r="G38" s="32"/>
-      <c r="H38" s="16"/>
-      <c r="I38" s="32"/>
+      <c r="H38" s="16">
+        <v>10</v>
+      </c>
+      <c r="I38" s="32" t="s">
+        <v>106</v>
+      </c>
       <c r="J38" s="16"/>
       <c r="K38" s="32"/>
     </row>
-    <row r="39" spans="1:11" ht="42.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="15" t="s">
-        <v>86</v>
-      </c>
-      <c r="B39" s="16">
-        <f>SUM(B34:B38)</f>
-        <v>87</v>
-      </c>
+    <row r="39" spans="1:11" ht="42.6" customHeight="1" thickBot="1">
+      <c r="A39" s="15"/>
+      <c r="B39" s="16"/>
       <c r="C39" s="32"/>
-      <c r="D39" s="16">
-        <f>SUM(D36:D38)</f>
-        <v>0</v>
-      </c>
+      <c r="D39" s="16"/>
       <c r="E39" s="32"/>
-      <c r="F39" s="16">
-        <f>SUM(F36:F38)</f>
-        <v>0</v>
-      </c>
+      <c r="F39" s="16"/>
       <c r="G39" s="32"/>
       <c r="H39" s="16">
-        <f>SUM(H36:H38)</f>
+        <v>0.75</v>
+      </c>
+      <c r="I39" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="J39" s="16"/>
+      <c r="K39" s="32"/>
+    </row>
+    <row r="40" spans="1:11" ht="42.6" customHeight="1" thickBot="1">
+      <c r="A40" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="B40" s="16">
+        <v>10</v>
+      </c>
+      <c r="C40" s="32" t="s">
+        <v>103</v>
+      </c>
+      <c r="D40" s="16"/>
+      <c r="E40" s="32"/>
+      <c r="F40" s="16"/>
+      <c r="G40" s="32"/>
+      <c r="H40" s="16">
+        <v>3</v>
+      </c>
+      <c r="I40" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="J40" s="16"/>
+      <c r="K40" s="32"/>
+    </row>
+    <row r="41" spans="1:11" ht="42.6" customHeight="1" thickBot="1">
+      <c r="A41" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="B41" s="16">
+        <f>SUM(B35:B40)</f>
+        <v>35.25</v>
+      </c>
+      <c r="C41" s="32"/>
+      <c r="D41" s="16">
+        <f>SUM(D36:D40)</f>
+        <v>10</v>
+      </c>
+      <c r="E41" s="32"/>
+      <c r="F41" s="16">
+        <f>SUM(F36:F40)</f>
         <v>0</v>
       </c>
-      <c r="I39" s="32"/>
-      <c r="J39" s="16">
-        <f>SUM(J36:J38)</f>
-        <v>0</v>
-      </c>
-      <c r="K39" s="32"/>
+      <c r="G41" s="32"/>
+      <c r="H41" s="16">
+        <f>SUM(H35:H40)</f>
+        <v>19</v>
+      </c>
+      <c r="I41" s="32"/>
+      <c r="J41" s="16">
+        <f>SUM(J35:J40)</f>
+        <v>5</v>
+      </c>
+      <c r="K41" s="32"/>
+    </row>
+    <row r="42" spans="1:11" ht="42.6" customHeight="1" thickBot="1">
+      <c r="A42" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B42" s="16">
+        <f>B41+B34+B28+D42</f>
+        <v>196</v>
+      </c>
+      <c r="D42" s="1">
+        <f>D41+D34+D28+D22</f>
+        <v>77.5</v>
+      </c>
+      <c r="F42" s="1">
+        <f>F41+F34+F28+F22</f>
+        <v>69.75</v>
+      </c>
+      <c r="H42" s="1">
+        <f>H41+H34+H28+H22</f>
+        <v>91.75</v>
+      </c>
+      <c r="J42" s="1">
+        <f>J41+J34+J28+J22</f>
+        <v>96.5</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="J1:K1"/>
     <mergeCell ref="A23:A24"/>
     <mergeCell ref="A29:A30"/>
     <mergeCell ref="A13:A14"/>
@@ -2363,11 +2415,6 @@
     <mergeCell ref="A6:A8"/>
     <mergeCell ref="A9:A12"/>
     <mergeCell ref="A25:A27"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="H1:I1"/>
-    <mergeCell ref="J1:K1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2375,24 +2422,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>